<commit_message>
Converting LunchMenu form html/java to xhtml/facelets/java
</commit_message>
<xml_diff>
--- a/src/main/resources/menu.xlsx
+++ b/src/main/resources/menu.xlsx
@@ -5,17 +5,17 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hanne\Desktop\javap2\home_page\src\main\java\com\example\home_page\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\arche\Desktop\Java\home_page\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77BECA0D-14D4-4FFF-814F-68DF972450C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F481F572-2817-41A0-AC2D-5FA649392294}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{D6EBB21D-5D0C-4B27-BB09-633ADB448E88}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" xr2:uid="{D6EBB21D-5D0C-4B27-BB09-633ADB448E88}"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029" refMode="R1C1"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>Måndag</t>
   </si>
@@ -81,6 +81,15 @@
   </si>
   <si>
     <t>Einars Köttbullar</t>
+  </si>
+  <si>
+    <t>Lördag</t>
+  </si>
+  <si>
+    <t>Grillad Ryggbiff</t>
+  </si>
+  <si>
+    <t>med pommes och hemmaslagen bea</t>
   </si>
 </sst>
 </file>
@@ -455,86 +464,101 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4757B843-85C6-4F6D-9DBC-0544945214A5}">
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="2" max="2" width="24.21875" customWidth="1"/>
-    <col min="3" max="3" width="113.44140625" customWidth="1"/>
+    <col min="2" max="2" width="24.19921875" customWidth="1"/>
+    <col min="3" max="3" width="113.46484375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="22.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:4" ht="22.8" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="2" spans="1:4" ht="16.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1">
+      <c r="D2" s="1">
         <v>100</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="1" t="s">
+    <row r="3" spans="1:4" ht="13.8" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="1">
+      <c r="D3" s="1">
         <v>120</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="1" t="s">
+    <row r="4" spans="1:4" ht="20.45" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A4" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B4" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="C4" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="1">
+      <c r="D4" s="1">
         <v>110</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="1" t="s">
+    <row r="5" spans="1:4" ht="16.8" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A5" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B5" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="C5" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D4" s="1">
+      <c r="D5" s="1">
         <v>100</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="1" t="s">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A6" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B6" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="C6" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D5" s="1">
+      <c r="D6" s="1">
         <v>130</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A7" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D7" s="1">
+        <v>190</v>
       </c>
     </row>
   </sheetData>

</xml_diff>